<commit_message>
removed midi cable link (wrong wiring)
</commit_message>
<xml_diff>
--- a/DODECA_MOUSER_BOM.xlsx
+++ b/DODECA_MOUSER_BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="147">
   <si>
     <t>DODECA</t>
   </si>
@@ -483,24 +483,31 @@
     </r>
   </si>
   <si>
+    <t>PCB SET</t>
+  </si>
+  <si>
+    <t>DUBDECA PANEL</t>
+  </si>
+  <si>
     <t>MIDI to stereo cable</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>https://www.amazon.com/DIN-Male-Playing-Electronic-Musical-Instrument/dp/B01KTFW7S8/ref=sr_1_2?ie=UTF8&amp;qid=1504146829&amp;sr=8-2&amp;keywords=midi+to+stereo</t>
-    </r>
-  </si>
-  <si>
     <t>10 pin euro power header</t>
   </si>
   <si>
     <t>Est Total Cost:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doubldeca = </t>
+  </si>
+  <si>
+    <t>Built Price</t>
+  </si>
+  <si>
+    <t>Build time</t>
+  </si>
+  <si>
+    <t>Rater per hour</t>
   </si>
 </sst>
 </file>
@@ -786,7 +793,13 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -876,7 +889,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -885,10 +898,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1143,7 +1156,13 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1447,7 +1466,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1456,10 +1475,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1710,7 +1729,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1719,14 +1738,14 @@
     <col min="1" max="1" width="26.4453" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.8672" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.4453" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.86719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.4453" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5781" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.80469" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.3828" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.4922" style="1" customWidth="1"/>
     <col min="7" max="7" width="54.7344" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1562" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.57812" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1719" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.15625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="40.1562" style="1" customWidth="1"/>
+    <col min="11" max="11" width="40.0938" style="1" customWidth="1"/>
     <col min="12" max="256" width="7.57812" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2838,11 +2857,14 @@
         <v>138</v>
       </c>
       <c r="H41" s="3"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" t="s" s="5">
-        <v>139</v>
-      </c>
+      <c r="I41" s="6">
+        <v>15</v>
+      </c>
+      <c r="J41" s="6">
+        <f>D41*I41</f>
+        <v>15</v>
+      </c>
+      <c r="K41" s="3"/>
     </row>
     <row r="42" ht="14.95" customHeight="1">
       <c r="A42" s="3"/>
@@ -2854,30 +2876,153 @@
       <c r="E42" s="3"/>
       <c r="F42" s="5"/>
       <c r="G42" t="s" s="5">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H42" s="3"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
+      <c r="I42" s="6">
+        <v>27</v>
+      </c>
+      <c r="J42" s="6">
+        <f>D42*I42</f>
+        <v>27</v>
+      </c>
+      <c r="K42" s="3"/>
     </row>
     <row r="43" ht="14.95" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="4"/>
+      <c r="D43" s="10">
+        <v>1</v>
+      </c>
       <c r="E43" s="3"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="3"/>
+      <c r="G43" t="s" s="5">
+        <v>140</v>
+      </c>
       <c r="H43" s="3"/>
-      <c r="I43" t="s" s="12">
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" ht="14.95" customHeight="1">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="10">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="5"/>
+      <c r="G44" t="s" s="5">
         <v>141</v>
       </c>
-      <c r="J43" s="6">
+      <c r="H44" s="3"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+    </row>
+    <row r="45" ht="14.95" customHeight="1">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" t="s" s="12">
+        <v>142</v>
+      </c>
+      <c r="J45" s="6">
         <f>SUM(J4:J39)</f>
         <v>54.45999999999999</v>
       </c>
-      <c r="K43" s="6"/>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" ht="14.95" customHeight="1">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" t="s" s="5">
+        <v>143</v>
+      </c>
+      <c r="J46" s="6">
+        <f>J45*2+(J41+J42)</f>
+        <v>150.92</v>
+      </c>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" ht="14.95" customHeight="1">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" t="s" s="5">
+        <v>144</v>
+      </c>
+      <c r="J47" s="6">
+        <v>275</v>
+      </c>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" ht="14.95" customHeight="1">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" t="s" s="5">
+        <v>145</v>
+      </c>
+      <c r="J48" s="6">
+        <f>J47-J46</f>
+        <v>124.08</v>
+      </c>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" ht="14.95" customHeight="1">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" t="s" s="5">
+        <v>146</v>
+      </c>
+      <c r="J49" s="6">
+        <f>J48/6</f>
+        <v>20.68</v>
+      </c>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" ht="14.95" customHeight="1">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2909,6 +3054,9 @@
     <hyperlink ref="H34" r:id="rId26" location="" tooltip="" display=""/>
     <hyperlink ref="H35" r:id="rId27" location="" tooltip="" display=""/>
     <hyperlink ref="H36" r:id="rId28" location="" tooltip="" display=""/>
+    <hyperlink ref="G38" r:id="rId29" location="" tooltip="" display=""/>
+    <hyperlink ref="K39" r:id="rId30" location="" tooltip="" display=""/>
+    <hyperlink ref="K40" r:id="rId31" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>

</xml_diff>